<commit_message>
Save-pre changes to expulsion timings
</commit_message>
<xml_diff>
--- a/ExperimentLog.xlsx
+++ b/ExperimentLog.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +25,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +47,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +72,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,13 +435,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -645,6 +655,2052 @@
       </c>
       <c r="X2" t="n">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>09:27:58</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-03-27</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>150</v>
+      </c>
+      <c r="I3" t="n">
+        <v>50</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>DPPC</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>96</v>
+      </c>
+      <c r="O3" t="n">
+        <v>80</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Lyso</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" t="n">
+        <v>40</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Chol</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
+        <v>20</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>09:29:59</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-03-27</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>150</v>
+      </c>
+      <c r="I4" t="n">
+        <v>50</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>DPPC</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>96</v>
+      </c>
+      <c r="O4" t="n">
+        <v>80</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Lyso</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S4" t="n">
+        <v>40</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Chol</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" t="n">
+        <v>20</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>140-FlowTestn/an/an/a</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10:49:02</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>140</v>
+      </c>
+      <c r="I5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.488275862068966</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>40</v>
+      </c>
+      <c r="P5" t="n">
+        <v>13.6023099137931</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10:54:10</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>140</v>
+      </c>
+      <c r="I6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1765517241379311</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>40</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4991633620689656</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10:54:48</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>140</v>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>60</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.02068965517241376</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>30</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.08181551724137819</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11:05:50</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>140</v>
+      </c>
+      <c r="I8" t="n">
+        <v>30</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>50</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.02137931034482762</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>40</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.08718060344827575</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11:06:28</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>140</v>
+      </c>
+      <c r="I9" t="n">
+        <v>30</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>60</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.03045977011494259</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>30</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.1097465517241372</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>11:08:39</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>140</v>
+      </c>
+      <c r="I10" t="n">
+        <v>30</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>50</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.02689655172413793</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>40</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.07691422413793099</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11:10:43</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>140</v>
+      </c>
+      <c r="I11" t="n">
+        <v>30</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>50</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.03310344827586206</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>40</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.09437112068965625</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>11:20:22</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>140</v>
+      </c>
+      <c r="I12" t="n">
+        <v>30</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>50</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.01724137931034477</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>40</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.06274094827586225</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>11:21:01</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H13" t="n">
+        <v>140</v>
+      </c>
+      <c r="I13" t="n">
+        <v>30</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>60</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.01551724137931032</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>30</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.08181551724137819</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>11:21:35</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>[1, 3]</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>140</v>
+      </c>
+      <c r="I14" t="n">
+        <v>30</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>70</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.01133004926108368</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>20</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.1339301724137925</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>11:22:07</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[1, 4]</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>140</v>
+      </c>
+      <c r="I15" t="n">
+        <v>30</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>80</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.009482758620689679</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>50</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.05967551724137877</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>140-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>11:22:34</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[1, 5]</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>140</v>
+      </c>
+      <c r="I16" t="n">
+        <v>30</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.01172413793103445</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>40</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.05924956896551663</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11:39:43</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>140</v>
+      </c>
+      <c r="I17" t="n">
+        <v>30</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>50</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.1717241379310344</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>40</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.6425176724137935</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>11:40:21</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>140</v>
+      </c>
+      <c r="I18" t="n">
+        <v>30</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>60</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.03850574712643677</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>30</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.1097465517241372</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11:41:33</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[1, 3]</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>140</v>
+      </c>
+      <c r="I19" t="n">
+        <v>30</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>70</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.009359605911330147</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>20</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.1618612068965516</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W19" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>11:42:08</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[1, 4]</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>140</v>
+      </c>
+      <c r="I20" t="n">
+        <v>30</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>80</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.009482758620689679</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>50</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.06526172413793048</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>11:42:38</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024-04-04</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[1, 5]</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H21" t="n">
+        <v>140</v>
+      </c>
+      <c r="I21" t="n">
+        <v>30</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>100</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.007586206896551744</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>40</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.05575818965517243</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Failed to Eq</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>15:26:55</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>140</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>50</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>50</v>
+      </c>
+      <c r="P22" t="n">
+        <v>7.487290000000001</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>50</v>
+      </c>
+      <c r="T22" t="n">
+        <v>7.487290000000001</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2.5-FlowTestnanana</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Failed to Eq</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>15:35:30</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>140</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>50</v>
+      </c>
+      <c r="L23" t="n">
+        <v>10.88896551724138</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>50</v>
+      </c>
+      <c r="P23" t="n">
+        <v>96.12922103448277</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="S23" t="n">
+        <v>50</v>
+      </c>
+      <c r="T23" t="n">
+        <v>20.75657206896551</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add interpolation and tuning
</commit_message>
<xml_diff>
--- a/ExperimentLog.xlsx
+++ b/ExperimentLog.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -3309,6 +3309,1319 @@
         <v>0.7330857758620691</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>09:29:30</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H30" t="n">
+        <v>120</v>
+      </c>
+      <c r="I30" t="n">
+        <v>50</v>
+      </c>
+      <c r="J30" t="n">
+        <v>29.00098133087158</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>50</v>
+      </c>
+      <c r="M30" t="n">
+        <v>2.124137931034483</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P30" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>1.26071</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>50</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.9339168965517243</v>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X30" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1.042847931034482</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>10:11:25</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H31" t="n">
+        <v>120</v>
+      </c>
+      <c r="I31" t="n">
+        <v>50</v>
+      </c>
+      <c r="J31" t="n">
+        <v>64.67762470245361</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L31" t="n">
+        <v>50</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1.256551724137931</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P31" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1.101503103448275</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>50</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.8361582758620688</v>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X31" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.763537586206896</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>10:12:21</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>[1, 3]</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H32" t="n">
+        <v>120</v>
+      </c>
+      <c r="I32" t="n">
+        <v>50</v>
+      </c>
+      <c r="J32" t="n">
+        <v>26.03447842597961</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L32" t="n">
+        <v>40</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.826724137931035</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>2.031878879310343</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T32" t="n">
+        <v>40</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1.08920646551724</v>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X32" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1.239335775862069</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>10:13:13</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>[1, 4]</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H33" t="n">
+        <v>120</v>
+      </c>
+      <c r="I33" t="n">
+        <v>50</v>
+      </c>
+      <c r="J33" t="n">
+        <v>31.4096953868866</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L33" t="n">
+        <v>60</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1.257471264367816</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P33" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.9258215517241375</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T33" t="n">
+        <v>60</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.7070284482758619</v>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X33" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.7396146551724132</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>10:14:01</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>[1, 5]</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H34" t="n">
+        <v>120</v>
+      </c>
+      <c r="I34" t="n">
+        <v>50</v>
+      </c>
+      <c r="J34" t="n">
+        <v>30.26472544670105</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>70</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1.16551724137931</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P34" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.7724036945812802</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T34" t="n">
+        <v>70</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.5429701970443349</v>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X34" t="n">
+        <v>70</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.6088076354679803</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Failed to Eq</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>10:44:43</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H35" t="n">
+        <v>120</v>
+      </c>
+      <c r="I35" t="n">
+        <v>50</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L35" t="n">
+        <v>50</v>
+      </c>
+      <c r="M35" t="n">
+        <v>2.520689655172414</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P35" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>7.051565862068966</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T35" t="n">
+        <v>50</v>
+      </c>
+      <c r="U35" t="n">
+        <v>6.604669310344828</v>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X35" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>6.694048620689656</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>10:50:40</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H36" t="n">
+        <v>120</v>
+      </c>
+      <c r="I36" t="n">
+        <v>50</v>
+      </c>
+      <c r="J36" t="n">
+        <v>32.52000260353088</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L36" t="n">
+        <v>50</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.02896551724137936</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P36" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.1183306896551724</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T36" t="n">
+        <v>50</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.101572068965517</v>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X36" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0.09039965517241327</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>10:56:36</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>[1, 2]</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H37" t="n">
+        <v>120</v>
+      </c>
+      <c r="I37" t="n">
+        <v>50</v>
+      </c>
+      <c r="J37" t="n">
+        <v>37.01172184944153</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
+        <v>50</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.03310344827586206</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.04087620689655211</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>50</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.05204862068965582</v>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X37" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0.04087620689655211</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>[1, 3]</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H38" t="n">
+        <v>120</v>
+      </c>
+      <c r="I38" t="n">
+        <v>50</v>
+      </c>
+      <c r="J38" t="n">
+        <v>28.42667031288147</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L38" t="n">
+        <v>40</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.06465517241379307</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.04877543103448261</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>40</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.05924956896551663</v>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X38" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0.05575818965517243</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>10:58:24</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>[1, 4]</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H39" t="n">
+        <v>120</v>
+      </c>
+      <c r="I39" t="n">
+        <v>50</v>
+      </c>
+      <c r="J39" t="n">
+        <v>28.78419852256775</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L39" t="n">
+        <v>60</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.04712643678160925</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P39" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.03779913793103518</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T39" t="n">
+        <v>60</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.03547155172413809</v>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X39" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0.05176465517241387</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>10:59:04</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>[1, 5]</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H40" t="n">
+        <v>120</v>
+      </c>
+      <c r="I40" t="n">
+        <v>50</v>
+      </c>
+      <c r="J40" t="n">
+        <v>21.44424200057983</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>70</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.0261083743842365</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P40" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.04956674876847294</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T40" t="n">
+        <v>70</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.03959137931034503</v>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X40" t="n">
+        <v>70</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0.03360615763546845</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>10:59:47</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>[1, 6]</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H41" t="n">
+        <v>120</v>
+      </c>
+      <c r="I41" t="n">
+        <v>50</v>
+      </c>
+      <c r="J41" t="n">
+        <v>28.24206376075745</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>80</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.03232758620689662</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P41" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.04268125000000023</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T41" t="n">
+        <v>80</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.0322071120689655</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X41" t="n">
+        <v>80</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0.0356984913793104</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0.3333333333333333-FlowTest150424nanana</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>11:01:11</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>[1, 7]</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H42" t="n">
+        <v>120</v>
+      </c>
+      <c r="I42" t="n">
+        <v>50</v>
+      </c>
+      <c r="J42" t="n">
+        <v>43.78574204444885</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>BufferX</t>
+        </is>
+      </c>
+      <c r="L42" t="n">
+        <v>30</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.04022988505747129</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Lipid1</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="P42" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.04387413793103541</v>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Lipid2</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="T42" t="n">
+        <v>30</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.1097465517241372</v>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>Lipid3</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="X42" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0.1376775862068965</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>